<commit_message>
Finished implementation of method extractColumns and associated others.
</commit_message>
<xml_diff>
--- a/tests/nabu/spreadsheet/resources/basic-excel-file.xlsx
+++ b/tests/nabu/spreadsheet/resources/basic-excel-file.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rgutierrez/GitHub/nabu-3/spreadsheet-utils/tests/nabu/spreadsheet/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7557EE1-1D17-2242-AAC4-582B193526F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65C28DA-5DB7-E546-B116-536A2881C353}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{68A98C51-1DDA-4F4D-A751-22B34B0BF22F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,10 +39,10 @@
     <t>Column 2</t>
   </si>
   <si>
-    <t>Cólùm 3</t>
+    <t>Test string</t>
   </si>
   <si>
-    <t>Test string</t>
+    <t>Cólùmn 3</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -411,7 +411,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -419,7 +419,7 @@
         <v>123</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <f>A2*3</f>

</xml_diff>

<commit_message>
Add support for indexed data
</commit_message>
<xml_diff>
--- a/tests/nabu/spreadsheet/resources/basic-excel-file.xlsx
+++ b/tests/nabu/spreadsheet/resources/basic-excel-file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rgutierrez/GitHub/nabu-3/spreadsheet-utils/tests/nabu/spreadsheet/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65C28DA-5DB7-E546-B116-536A2881C353}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78C04A6-3F63-E141-B6EF-AB71FF47CD7F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1860" windowWidth="28040" windowHeight="17440" xr2:uid="{68A98C51-1DDA-4F4D-A751-22B34B0BF22F}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Column 1</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Cólùmn 3</t>
+  </si>
+  <si>
+    <t>Other test</t>
+  </si>
+  <si>
+    <t>More tests data</t>
   </si>
 </sst>
 </file>
@@ -395,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1457AA96-98EC-AA47-9F4A-1BBE8C9822FA}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -426,6 +432,28 @@
         <v>369</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>456</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>789</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>147</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>